<commit_message>
runoff depth and UHI.xlsx
</commit_message>
<xml_diff>
--- a/runoff depth and UHI.xlsx
+++ b/runoff depth and UHI.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48BE8EBC-8D15-4450-9452-CBB30D68C8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\ET calculation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B32AC1-1FEF-4E22-B85F-A9C67EE0A0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="math" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>catchment area</t>
   </si>
@@ -205,12 +210,15 @@
   <si>
     <t>y = y1 + ((x – x1) / (x2 – x1)) * (y2 – y1), </t>
   </si>
+  <si>
+    <t>5 cm rainfall runoff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -311,7 +319,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2103,6 +2110,12 @@
               <c:f>'UH Math II'!$F$3:$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 cm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6-H unit hydrograph</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>1 cm rainfall-runoff</c:v>
                 </c:pt>
@@ -2279,9 +2292,6 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3 cm 6 H</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12 H 5 cm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7044,7 +7054,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="5" name="">
+            <xdr14:cNvPr id="5" name="Ink 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30699DAF-9CC4-4BD2-83EA-9A6B0FCD250C}"/>
@@ -7120,7 +7130,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="3" name="">
+            <xdr14:cNvPr id="3" name="Ink 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{560FE656-7827-4B35-AE7E-1FA6797AF590}"/>
@@ -7185,7 +7195,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="4" name="">
+            <xdr14:cNvPr id="4" name="Ink 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA8D8378-F3ED-49FC-86E9-EEB2C16FD686}"/>
@@ -7256,7 +7266,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="6" name="">
+            <xdr14:cNvPr id="6" name="Ink 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74443C4F-E833-4D02-ADF0-99FE3B59B885}"/>
@@ -7327,7 +7337,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="7" name="">
+            <xdr14:cNvPr id="7" name="Ink 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DA8FCF-ED73-44CF-AA65-B207775E0B7F}"/>
@@ -7398,7 +7408,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="8" name="">
+            <xdr14:cNvPr id="8" name="Ink 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B096C678-7A32-4BFA-94B8-EE5549ADB676}"/>
@@ -7469,7 +7479,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="9" name="">
+            <xdr14:cNvPr id="9" name="Ink 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE0F5329-D0FE-4119-BC1D-81C7FB40B3E5}"/>
@@ -7540,7 +7550,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="10" name="">
+            <xdr14:cNvPr id="10" name="Ink 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3D56B22-0E5A-457D-9928-75DF9559831C}"/>
@@ -7611,7 +7621,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="11" name="">
+            <xdr14:cNvPr id="11" name="Ink 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFB38A58-597B-42D4-96CE-FB26D0114484}"/>
@@ -7672,16 +7682,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7719,11 +7729,11 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="9" name="">
+            <xdr14:cNvPr id="9" name="Ink 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E86DCA6A-4D31-4671-8910-01B205800BB0}"/>
@@ -7742,7 +7752,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="">
@@ -7843,7 +7853,7 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="6" name="">
+            <xdr14:cNvPr id="6" name="Ink 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD34492C-A9A6-4E80-BCF6-8E230D18726C}"/>
@@ -8146,6 +8156,7 @@
           <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
         </inkml:channelProperties>
       </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-10-01T18:27:01.279"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.1" units="cm"/>
@@ -8153,10 +8164,10 @@
       <inkml:brushProperty name="color" value="#AB008B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">25070 6517 16383 0 0,'0'0'0'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="0.58">29540 3211 16383 0 0,'0'0'0'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="0.6">29540 3211 16383 0 0,'0'0'0'0'0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="0.62">29540 3211 16383 0 0,'0'0'0'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">25070 6412 16383 0 0,'0'0'0'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2.14748E7">29541 3211 16383 0 0,'0'0'0'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2.14748E7">29541 3211 16383 0 0,'0'0'0'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2.14748E7">29541 3211 16383 0 0,'0'0'0'0'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8188,13 +8199,13 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">24386 5142 16383 0 0,'-15'-3'0'0'0,"-17"-7"0"0"0,-27-14 0 0 0,-10-6 0 0 0,-16-15 0 0 0,-22-19 0 0 0,-7-10 0 0 0,-5-1 0 0 0,3 2 0 0 0,14 12 0 0 0,10 9 0 0 0,15 8 0 0 0,12 5 0 0 0,1 4 0 0 0,8 1 0 0 0,-3-2 0 0 0,-13-4 0 0 0,-22-5 0 0 0,-15-6 0 0 0,-10-3 0 0 0,-7-5 0 0 0,10 1 0 0 0,7 3 0 0 0,15 9 0 0 0,18 11 0 0 0,16 7 0 0 0,15 9 0 0 0,7 5 0 0 0,6 1 0 0 0,-4 1 0 0 0,6-2 0 0 0,-3-3 0 0 0,0-6 0 0 0,-2-4 0 0 0,0-1 0 0 0,-1-2 0 0 0,-5 2 0 0 0,-6-1 0 0 0,0 2 0 0 0,2-4 0 0 0,-13-3 0 0 0,-5-1 0 0 0,-11-3 0 0 0,-6-8 0 0 0,-6-2 0 0 0,-9-2 0 0 0,0 2 0 0 0,10 3 0 0 0,17 9 0 0 0,13 10 0 0 0,5 8 0 0 0,1 6 0 0 0,3 5 0 0 0,4-5 0 0 0,3-1 0 0 0,-11-1 0 0 0,-2 3 0 0 0,-7-4 0 0 0,0 0 0 0 0,4 1 0 0 0,6 0 0 0 0,5 1 0 0 0,7 1 0 0 0,6 2 0 0 0,7 2 0 0 0,-15 1 0 0 0,-6-3 0 0 0,-5 1 0 0 0,1-4 0 0 0,-4 0 0 0 0,-5 3 0 0 0,-1 2 0 0 0,3 3 0 0 0,5 2 0 0 0,-4-4 0 0 0,5-1 0 0 0,-1-2 0 0 0,-2 0 0 0 0,1 3 0 0 0,-8-1 0 0 0,-1-3 0 0 0,-9 2 0 0 0,2-2 0 0 0,3 2 0 0 0,-5 2 0 0 0,0 2 0 0 0,0 3 0 0 0,-3 0 0 0 0,-1 2 0 0 0,-6 0 0 0 0,5 0 0 0 0,-3 1 0 0 0,2-1 0 0 0,9 1 0 0 0,9-1 0 0 0,9 0 0 0 0,7 0 0 0 0,7 0 0 0 0,4 6 0 0 0,1 5 0 0 0,3 4 0 0 0,-1 4 0 0 0,-1 1 0 0 0,-4 1 0 0 0,-9 4 0 0 0,2 1 0 0 0,-3-2 0 0 0,-7 5 0 0 0,0 6 0 0 0,4 3 0 0 0,-1 5 0 0 0,1 9 0 0 0,6 2 0 0 0,3 4 0 0 0,8-2 0 0 0,6-5 0 0 0,4 2 0 0 0,-4 3 0 0 0,-1-2 0 0 0,4-3 0 0 0,5-3 0 0 0,5-5 0 0 0,4-8 0 0 0,1 6 0 0 0,0-2 0 0 0,2 2 0 0 0,-2 30 0 0 0,-1 21 0 0 0,-4 39 0 0 0,-1 23 0 0 0,1-11 0 0 0,3-16 0 0 0,2-24 0 0 0,3-24 0 0 0,0-19 0 0 0,2-14 0 0 0,0-12 0 0 0,1-2 0 0 0,-1 11 0 0 0,0 7 0 0 0,1 29 0 0 0,5 18 0 0 0,5 8 0 0 0,4 4 0 0 0,8 4 0 0 0,0-10 0 0 0,-1-6 0 0 0,-1-13 0 0 0,8-8 0 0 0,2-12 0 0 0,14-4 0 0 0,14-1 0 0 0,0-4 0 0 0,-1 1 0 0 0,-4 2 0 0 0,-6 10 0 0 0,-2-1 0 0 0,-2 0 0 0 0,-3 1 0 0 0,-3 1 0 0 0,5 12 0 0 0,4 2 0 0 0,-4-5 0 0 0,-5-12 0 0 0,-10-14 0 0 0,-3-11 0 0 0,-3-5 0 0 0,7-4 0 0 0,7 0 0 0 0,7-4 0 0 0,16 0 0 0 0,11-1 0 0 0,3-3 0 0 0,3-3 0 0 0,13-1 0 0 0,-5-5 0 0 0,-3 5 0 0 0,-8 2 0 0 0,-12-1 0 0 0,-6 0 0 0 0,-10-3 0 0 0,-3-3 0 0 0,0-3 0 0 0,1-1 0 0 0,4-2 0 0 0,7-3 0 0 0,2-2 0 0 0,2-2 0 0 0,-2-2 0 0 0,5 3 0 0 0,-3 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,0-1 0 0 0,-1-1 0 0 0,-5 0 0 0 0,6-3 0 0 0,-3-1 0 0 0,5-12 0 0 0,0-3 0 0 0,-3 2 0 0 0,7 3 0 0 0,4 1 0 0 0,5 4 0 0 0,-3 2 0 0 0,-7 0 0 0 0,3-2 0 0 0,-3 0 0 0 0,-3 0 0 0 0,-3 0 0 0 0,-2-1 0 0 0,-3 2 0 0 0,3-2 0 0 0,-4 2 0 0 0,6 1 0 0 0,3 3 0 0 0,7 1 0 0 0,1-1 0 0 0,6 0 0 0 0,-1 0 0 0 0,-4-5 0 0 0,-2 0 0 0 0,-4 0 0 0 0,-6 3 0 0 0,-6-2 0 0 0,-4 2 0 0 0,-6-3 0 0 0,6 2 0 0 0,3 1 0 0 0,2 2 0 0 0,9 2 0 0 0,4-3 0 0 0,-1 1 0 0 0,-6-3 0 0 0,8-12 0 0 0,-4-2 0 0 0,-2-1 0 0 0,-8 3 0 0 0,2 2 0 0 0,-5 4 0 0 0,3 1 0 0 0,7 2 0 0 0,12 1 0 0 0,11-2 0 0 0,-2 1 0 0 0,5-3 0 0 0,-9-1 0 0 0,-5 1 0 0 0,-7 1 0 0 0,-8 0 0 0 0,-8 0 0 0 0,-4-2 0 0 0,6-1 0 0 0,3-2 0 0 0,-3 0 0 0 0,9 0 0 0 0,9-7 0 0 0,19-2 0 0 0,3 0 0 0 0,5-4 0 0 0,12 0 0 0 0,6 5 0 0 0,5 1 0 0 0,-10 1 0 0 0,-14 2 0 0 0,-15 4 0 0 0,-6 6 0 0 0,3-3 0 0 0,-4 3 0 0 0,11-4 0 0 0,7 1 0 0 0,5 3 0 0 0,-7 3 0 0 0,-8 3 0 0 0,-10 2 0 0 0,-2 2 0 0 0,-4 1 0 0 0,-4 1 0 0 0,-10-1 0 0 0,-1 1 0 0 0,-4 0 0 0 0,-4-1 0 0 0,3 0 0 0 0,0 0 0 0 0,4 0 0 0 0,-1 0 0 0 0,21 0 0 0 0,-15 0 0 0 0,-24 0 0 0 0,-41-12 0 0 0,-22-4 0 0 0,-65-14 0 0 0,-38-11 0 0 0,-49-26 0 0 0,3-1 0 0 0,6-13 0 0 0,26 4 0 0 0,39 12 0 0 0,35 12 0 0 0,24 8 0 0 0,-3-12 0 0 0,-13-15 0 0 0,-11-15 0 0 0,8 1 0 0 0,14 14 0 0 0,6 12 0 0 0,-6 0 0 0 0,4 10 0 0 0,11 11 0 0 0,11 9 0 0 0,9 4 0 0 0,-1-3 0 0 0,0 4 0 0 0,3 2 0 0 0,6 0 0 0 0,-2-2 0 0 0,3-1 0 0 0,-1 6 0 0 0,3 1 0 0 0,2 6 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">25709 6394 16383 0 0,'-3'0'0'0'0,"-1"3"0"0"0,-24 7 0 0 0,-37 8 0 0 0,-14 4 0 0 0,-16-3 0 0 0,-42-9 0 0 0,1-7 0 0 0,2-7 0 0 0,15-3 0 0 0,3-6 0 0 0,16-1 0 0 0,22 2 0 0 0,21 3 0 0 0,8 0 0 0 0,7 2 0 0 0,-2 2 0 0 0,-3 1 0 0 0,-10 2 0 0 0,-11 1 0 0 0,-7-2 0 0 0,-10-3 0 0 0,-4-5 0 0 0,2 1 0 0 0,10-5 0 0 0,5 1 0 0 0,10-4 0 0 0,3 2 0 0 0,8 3 0 0 0,-7-2 0 0 0,-16-8 0 0 0,-13-2 0 0 0,-18-7 0 0 0,-10 0 0 0 0,-18-4 0 0 0,-8-5 0 0 0,9-4 0 0 0,14-4 0 0 0,10 3 0 0 0,10 2 0 0 0,5-2 0 0 0,-3-2 0 0 0,-7-2 0 0 0,0 6 0 0 0,-7-3 0 0 0,-17-3 0 0 0,-3 0 0 0 0,3 4 0 0 0,21 10 0 0 0,15 5 0 0 0,18 9 0 0 0,6 1 0 0 0,6 4 0 0 0,9 6 0 0 0,12 4 0 0 0,-30-3 0 0 0,-9 1 0 0 0,-18-2 0 0 0,-2 2 0 0 0,-2-7 0 0 0,5-1 0 0 0,6 0 0 0 0,13 2 0 0 0,3 1 0 0 0,10 0 0 0 0,3-1 0 0 0,-9-3 0 0 0,1-3 0 0 0,-2 1 0 0 0,-1-1 0 0 0,5 1 0 0 0,-1 1 0 0 0,3-2 0 0 0,-3-4 0 0 0,4-1 0 0 0,-5 2 0 0 0,3 1 0 0 0,7 2 0 0 0,10 4 0 0 0,8 3 0 0 0,8 3 0 0 0,3 0 0 0 0,7 0 0 0 0,-5-2 0 0 0,-9-4 0 0 0,-8-3 0 0 0,-5-1 0 0 0,-6-2 0 0 0,1-1 0 0 0,6 4 0 0 0,9 5 0 0 0,8 5 0 0 0,3 5 0 0 0,1 3 0 0 0,-3 1 0 0 0,-4 2 0 0 0,2 0 0 0 0,4 0 0 0 0,3 0 0 0 0,4-1 0 0 0,-7 1 0 0 0,-2-1 0 0 0,5 0 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">19306 4119 16383 0 0,'12'12'0'0'0,"10"7"0"0"0,4 0 0 0 0,-2 0 0 0 0,-6 0 0 0 0,-2-4 0 0 0,-1-1 0 0 0,0 3 0 0 0,0-1 0 0 0,1 2 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 2 0 0 0,-2-3 0 0 0,1-1 0 0 0,-2-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,1 1 0 0 0,7 9 0 0 0,6 6 0 0 0,2 1 0 0 0,-1 4 0 0 0,-3 1 0 0 0,-2 1 0 0 0,0 2 0 0 0,0-3 0 0 0,-1-1 0 0 0,-1-2 0 0 0,1 3 0 0 0,-2-2 0 0 0,1-2 0 0 0,-4-3 0 0 0,0-4 0 0 0,-4-4 0 0 0,-2 1 0 0 0,2-4 0 0 0,3 0 0 0 0,3-3 0 0 0,-2-1 0 0 0,-4 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,6 1 0 0 0,1-1 0 0 0,-4-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">20840 4436 16383 0 0,'12'0'0'0'0,"7"0"0"0"0,4 0 0 0 0,-3 3 0 0 0,1 4 0 0 0,1 4 0 0 0,-1 0 0 0 0,-1 4 0 0 0,8 20 0 0 0,6 11 0 0 0,-1 3 0 0 0,-5 0 0 0 0,-2-3 0 0 0,1-1 0 0 0,-1-1 0 0 0,-6-5 0 0 0,7 8 0 0 0,1 0 0 0 0,-4-6 0 0 0,0 0 0 0 0,-1-5 0 0 0,-4-5 0 0 0,-6-1 0 0 0,-2-7 0 0 0,0-1 0 0 0,-2-1 0 0 0,1 2 0 0 0,5 9 0 0 0,-1 2 0 0 0,7 10 0 0 0,-1 1 0 0 0,-3-5 0 0 0,1 19 0 0 0,-2-2 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">19429 5600 16383 0 0,'9'0'0'0'0,"6"0"0"0"0,4 0 0 0 0,1 0 0 0 0,3 0 0 0 0,4 0 0 0 0,3 0 0 0 0,0 0 0 0 0,1 0 0 0 0,3 0 0 0 0,3 0 0 0 0,4 0 0 0 0,-3-3 0 0 0,-1-1 0 0 0,-4 1 0 0 0,-4-1 0 0 0,1 2 0 0 0,-1 1 0 0 0,-3 0 0 0 0,-2 1 0 0 0,0-3 0 0 0,3-1 0 0 0,-1 0 0 0 0,-2 2 0 0 0,-1 0 0 0 0,-3-3 0 0 0,-3-2 0 0 0,0-1 0 0 0,1 1 0 0 0,6-1 0 0 0,5 0 0 0 0,-2-1 0 0 0,-1 2 0 0 0,-3-3 0 0 0,-4-1 0 0 0,5-2 0 0 0,1 1 0 0 0,-1 2 0 0 0,1 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,-3 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 2 0 0 0,-4-1 0 0 0,-1 1 0 0 0,-2-2 0 0 0,-2 0 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">20488 6429 16383 0 0,'3'0'0'0'0,"10"0"0"0"0,17 0 0 0 0,14 0 0 0 0,4 0 0 0 0,1 0 0 0 0,-3 0 0 0 0,-2 0 0 0 0,-7 0 0 0 0,-2 0 0 0 0,-6 0 0 0 0,0 0 0 0 0,6 0 0 0 0,6 0 0 0 0,5 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,7 0 0 0 0,4 0 0 0 0,1-3 0 0 0,-6-1 0 0 0,-6 1 0 0 0,-8 0 0 0 0,-5-3 0 0 0,-1 1 0 0 0,-3 0 0 0 0,1-1 0 0 0,3-3 0 0 0,2-3 0 0 0,0-2 0 0 0,0 0 0 0 0,-2 4 0 0 0,-1 0 0 0 0,0-1 0 0 0,-3-2 0 0 0,1 1 0 0 0,-6 0 0 0 0,-1-1 0 0 0,-3-1 0 0 0,-4 1 0 0 0,3 3 0 0 0,4-5 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 2 0 0 0,-1 1 0 0 0,-5 0 0 0 0,-1-2 0 0 0,-1 3 0 0 0,4-1 0 0 0,-2 0 0 0 0,0 2 0 0 0,0 2 0 0 0,3 0 0 0 0,-1-1 0 0 0,-2-2 0 0 0,-2-2 0 0 0,-1 1 0 0 0,0 3 0 0 0,4-3 0 0 0,2-2 0 0 0,1 2 0 0 0,0-4 0 0 0,-1 2 0 0 0,-3 0 0 0 0,-4 3 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">26132 6341 16383 0 0,'-6'0'0'0'0,"-8"3"0"0"0,-5 1 0 0 0,-1 3 0 0 0,-5 9 0 0 0,4 8 0 0 0,4 24 0 0 0,5 15 0 0 0,8 4 0 0 0,10-10 0 0 0,8-15 0 0 0,1-11 0 0 0,4-11 0 0 0,2-9 0 0 0,0-6 0 0 0,0-5 0 0 0,-1-1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,1-6 0 0 0,-2-2 0 0 0,1-4 0 0 0,-4-4 0 0 0,0-1 0 0 0,0-3 0 0 0,-3-5 0 0 0,-3 0 0 0 0,-2-8 0 0 0,-3-3 0 0 0,-5 4 0 0 0,-4 8 0 0 0,-6 8 0 0 0,-8 8 0 0 0,-5 5 0 0 0,0 4 0 0 0,0 1 0 0 0,2 2 0 0 0,2 0 0 0 0,1-1 0 0 0,1 0 0 0 0,5 6 0 0 0,3 4 0 0 0,1 7 0 0 0,0 3 0 0 0,1 1 0 0 0,8 12 0 0 0,16 12 0 0 0,6 1 0 0 0,2-7 0 0 0,4-11 0 0 0,2-10 0 0 0,0-8 0 0 0,-2-6 0 0 0,-6-7 0 0 0,-3-3 0 0 0,-2-10 0 0 0,-4-11 0 0 0,6-11 0 0 0,-1-1 0 0 0,-3 2 0 0 0,-4 5 0 0 0,-4 4 0 0 0,1-2 0 0 0,-2-2 0 0 0,-1 1 0 0 0,-2 3 0 0 0,-3 5 0 0 0,-5 8 0 0 0,-8 5 0 0 0,-4 5 0 0 0,-5 2 0 0 0,-2 2 0 0 0,-2 1 0 0 0,0 1 0 0 0,1 2 0 0 0,3 1 0 0 0,5 2 0 0 0,0 4 0 0 0,-1 8 0 0 0,1 4 0 0 0,3 1 0 0 0,4 24 0 0 0,19 25 0 0 0,29 17 0 0 0,17-3 0 0 0,6-17 0 0 0,-5-20 0 0 0,-9-18 0 0 0,-8-15 0 0 0,-9-10 0 0 0,-8-10 0 0 0,-3-7 0 0 0,-4-7 0 0 0,-4-5 0 0 0,-4-7 0 0 0,0 1 0 0 0,-1-3 0 0 0,-1-6 0 0 0,1 1 0 0 0,0 3 0 0 0,0 5 0 0 0,-5-9 0 0 0,-5 3 0 0 0,-5 3 0 0 0,-6 8 0 0 0,-7 7 0 0 0,-8 7 0 0 0,-6 5 0 0 0,2 2 0 0 0,3 3 0 0 0,4 0 0 0 0,1 0 0 0 0,2 4 0 0 0,2 6 0 0 0,5 4 0 0 0,3 3 0 0 0,3 2 0 0 0,11 8 0 0 0,20 13 0 0 0,9-2 0 0 0,4-7 0 0 0,-4-8 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">24395 5565 16383 0 0,'-15'-4'0'0'0,"-17"-8"0"0"0,-27-16 0 0 0,-10-8 0 0 0,-16-17 0 0 0,-22-23 0 0 0,-7-12 0 0 0,-6-1 0 0 0,4 2 0 0 0,14 15 0 0 0,10 10 0 0 0,15 10 0 0 0,12 6 0 0 0,1 4 0 0 0,8 2 0 0 0,-3-3 0 0 0,-13-4 0 0 0,-23-7 0 0 0,-14-6 0 0 0,-10-4 0 0 0,-7-7 0 0 0,10 3 0 0 0,7 2 0 0 0,14 12 0 0 0,19 12 0 0 0,16 9 0 0 0,15 10 0 0 0,7 7 0 0 0,6 0 0 0 0,-4 2 0 0 0,6-3 0 0 0,-3-3 0 0 0,0-7 0 0 0,-2-5 0 0 0,0-1 0 0 0,-1-3 0 0 0,-5 3 0 0 0,-6-2 0 0 0,0 3 0 0 0,2-4 0 0 0,-13-5 0 0 0,-6 0 0 0 0,-10-4 0 0 0,-6-10 0 0 0,-6-2 0 0 0,-9-2 0 0 0,0 2 0 0 0,10 3 0 0 0,17 11 0 0 0,13 13 0 0 0,5 8 0 0 0,0 8 0 0 0,4 6 0 0 0,4-7 0 0 0,3 0 0 0 0,-11-2 0 0 0,-2 4 0 0 0,-7-4 0 0 0,0-1 0 0 0,4 1 0 0 0,6 0 0 0 0,5 2 0 0 0,7 1 0 0 0,6 2 0 0 0,7 2 0 0 0,-15 2 0 0 0,-6-4 0 0 0,-5 2 0 0 0,0-6 0 0 0,-3 1 0 0 0,-5 3 0 0 0,-1 2 0 0 0,3 4 0 0 0,5 3 0 0 0,-4-5 0 0 0,5-2 0 0 0,-1-2 0 0 0,-2 0 0 0 0,1 4 0 0 0,-8-2 0 0 0,-1-3 0 0 0,-9 3 0 0 0,1-3 0 0 0,4 2 0 0 0,-5 3 0 0 0,0 2 0 0 0,0 3 0 0 0,-3 1 0 0 0,-1 2 0 0 0,-6 0 0 0 0,5 0 0 0 0,-3 1 0 0 0,1-1 0 0 0,10 1 0 0 0,9-1 0 0 0,9 0 0 0 0,7 0 0 0 0,7 0 0 0 0,4 7 0 0 0,1 7 0 0 0,3 3 0 0 0,-1 6 0 0 0,-1 1 0 0 0,-4 1 0 0 0,-9 4 0 0 0,2 2 0 0 0,-3-2 0 0 0,-7 5 0 0 0,0 8 0 0 0,4 3 0 0 0,-2 6 0 0 0,2 10 0 0 0,6 4 0 0 0,3 3 0 0 0,8-1 0 0 0,6-7 0 0 0,4 3 0 0 0,-4 4 0 0 0,-1-3 0 0 0,4-4 0 0 0,5-3 0 0 0,5-5 0 0 0,4-11 0 0 0,1 8 0 0 0,0-3 0 0 0,2 3 0 0 0,-2 35 0 0 0,-1 25 0 0 0,-4 47 0 0 0,-1 27 0 0 0,1-14 0 0 0,3-18 0 0 0,2-29 0 0 0,3-28 0 0 0,0-23 0 0 0,2-16 0 0 0,0-15 0 0 0,1-2 0 0 0,-1 13 0 0 0,0 9 0 0 0,1 33 0 0 0,5 23 0 0 0,5 8 0 0 0,4 6 0 0 0,8 4 0 0 0,0-12 0 0 0,-1-7 0 0 0,-1-15 0 0 0,8-10 0 0 0,2-14 0 0 0,14-5 0 0 0,14-1 0 0 0,0-4 0 0 0,0 0 0 0 0,-5 3 0 0 0,-6 12 0 0 0,-2-2 0 0 0,-2 1 0 0 0,-3 1 0 0 0,-3 0 0 0 0,5 16 0 0 0,4 1 0 0 0,-4-5 0 0 0,-5-15 0 0 0,-10-16 0 0 0,-3-14 0 0 0,-3-5 0 0 0,7-5 0 0 0,7 0 0 0 0,7-5 0 0 0,16 1 0 0 0,12-2 0 0 0,2-4 0 0 0,3-3 0 0 0,13-1 0 0 0,-5-6 0 0 0,-3 5 0 0 0,-8 4 0 0 0,-12-3 0 0 0,-6 1 0 0 0,-10-3 0 0 0,-3-4 0 0 0,0-4 0 0 0,2-1 0 0 0,3-2 0 0 0,7-4 0 0 0,2-3 0 0 0,2-1 0 0 0,-2-3 0 0 0,5 3 0 0 0,-3 2 0 0 0,1-1 0 0 0,0-1 0 0 0,1 0 0 0 0,0-2 0 0 0,-1-1 0 0 0,-4 0 0 0 0,5-4 0 0 0,-3 0 0 0 0,5-15 0 0 0,0-4 0 0 0,-3 3 0 0 0,7 3 0 0 0,4 2 0 0 0,5 4 0 0 0,-3 3 0 0 0,-7-1 0 0 0,3-1 0 0 0,-2-1 0 0 0,-4 0 0 0 0,-3 1 0 0 0,-2-2 0 0 0,-3 2 0 0 0,3-2 0 0 0,-4 3 0 0 0,6 1 0 0 0,3 3 0 0 0,7 1 0 0 0,1 0 0 0 0,6-1 0 0 0,0 0 0 0 0,-5-6 0 0 0,-2 1 0 0 0,-4-1 0 0 0,-6 4 0 0 0,-6-3 0 0 0,-4 3 0 0 0,-6-3 0 0 0,6 1 0 0 0,3 2 0 0 0,2 2 0 0 0,9 3 0 0 0,4-4 0 0 0,0 1 0 0 0,-7-3 0 0 0,8-14 0 0 0,-4-3 0 0 0,-2-2 0 0 0,-8 5 0 0 0,2 2 0 0 0,-5 4 0 0 0,3 2 0 0 0,7 2 0 0 0,12 1 0 0 0,11-2 0 0 0,-1 2 0 0 0,4-5 0 0 0,-9 0 0 0 0,-5 0 0 0 0,-7 2 0 0 0,-8 0 0 0 0,-8-1 0 0 0,-4-1 0 0 0,6-2 0 0 0,3-2 0 0 0,-3 0 0 0 0,9-1 0 0 0,10-7 0 0 0,18-3 0 0 0,3 0 0 0 0,5-4 0 0 0,12-1 0 0 0,6 6 0 0 0,5 2 0 0 0,-10 0 0 0 0,-13 4 0 0 0,-16 3 0 0 0,-6 8 0 0 0,3-3 0 0 0,-4 3 0 0 0,11-5 0 0 0,7 1 0 0 0,5 4 0 0 0,-7 4 0 0 0,-7 3 0 0 0,-11 2 0 0 0,-2 3 0 0 0,-4 1 0 0 0,-4 1 0 0 0,-10-1 0 0 0,-1 1 0 0 0,-4 1 0 0 0,-4-2 0 0 0,3 0 0 0 0,0 0 0 0 0,4 0 0 0 0,-1 0 0 0 0,22 0 0 0 0,-16 0 0 0 0,-24 0 0 0 0,-41-15 0 0 0,-22-4 0 0 0,-66-16 0 0 0,-37-14 0 0 0,-49-31 0 0 0,3 0 0 0 0,6-16 0 0 0,25 4 0 0 0,40 15 0 0 0,35 14 0 0 0,24 10 0 0 0,-3-15 0 0 0,-13-17 0 0 0,-11-19 0 0 0,8 2 0 0 0,14 17 0 0 0,6 13 0 0 0,-6 1 0 0 0,3 12 0 0 0,12 13 0 0 0,11 10 0 0 0,9 5 0 0 0,-1-3 0 0 0,0 4 0 0 0,3 3 0 0 0,6-1 0 0 0,-2-1 0 0 0,3-2 0 0 0,-1 7 0 0 0,3 2 0 0 0,2 6 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">25720 7051 16383 0 0,'-3'0'0'0'0,"-1"4"0"0"0,-24 8 0 0 0,-37 9 0 0 0,-14 5 0 0 0,-16-3 0 0 0,-43-12 0 0 0,2-7 0 0 0,2-9 0 0 0,15-3 0 0 0,3-7 0 0 0,16-2 0 0 0,22 3 0 0 0,20 3 0 0 0,9 0 0 0 0,7 3 0 0 0,-2 2 0 0 0,-3 1 0 0 0,-10 3 0 0 0,-11 1 0 0 0,-7-3 0 0 0,-10-3 0 0 0,-4-6 0 0 0,2 1 0 0 0,9-6 0 0 0,6 2 0 0 0,10-6 0 0 0,3 3 0 0 0,8 4 0 0 0,-7-3 0 0 0,-16-9 0 0 0,-13-3 0 0 0,-18-8 0 0 0,-10 0 0 0 0,-19-5 0 0 0,-7-5 0 0 0,9-6 0 0 0,14-4 0 0 0,10 4 0 0 0,10 1 0 0 0,5-1 0 0 0,-4-3 0 0 0,-6-3 0 0 0,0 8 0 0 0,-7-4 0 0 0,-17-3 0 0 0,-3 0 0 0 0,2 4 0 0 0,22 12 0 0 0,15 6 0 0 0,18 11 0 0 0,6 1 0 0 0,6 5 0 0 0,9 7 0 0 0,12 5 0 0 0,-30-4 0 0 0,-9 1 0 0 0,-18-2 0 0 0,-3 3 0 0 0,-1-9 0 0 0,5-2 0 0 0,6 1 0 0 0,13 2 0 0 0,3 2 0 0 0,10-1 0 0 0,3-1 0 0 0,-9-3 0 0 0,0-4 0 0 0,-1 1 0 0 0,-1-1 0 0 0,5 2 0 0 0,-1 0 0 0 0,3-2 0 0 0,-3-4 0 0 0,4-2 0 0 0,-5 2 0 0 0,3 2 0 0 0,7 2 0 0 0,10 5 0 0 0,7 3 0 0 0,9 4 0 0 0,3 0 0 0 0,7 0 0 0 0,-5-2 0 0 0,-9-6 0 0 0,-8-2 0 0 0,-5-2 0 0 0,-6-3 0 0 0,1 0 0 0 0,6 4 0 0 0,9 6 0 0 0,8 6 0 0 0,3 7 0 0 0,1 2 0 0 0,-3 2 0 0 0,-4 2 0 0 0,2 0 0 0 0,4 1 0 0 0,3-1 0 0 0,4-1 0 0 0,-8 1 0 0 0,-1-1 0 0 0,5 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">19309 4350 16383 0 0,'12'15'0'0'0,"10"7"0"0"0,4 1 0 0 0,-2-1 0 0 0,-6 1 0 0 0,-2-5 0 0 0,-1-2 0 0 0,0 5 0 0 0,0-2 0 0 0,1 2 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 3 0 0 0,-2-4 0 0 0,1-1 0 0 0,-2-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,1 1 0 0 0,7 11 0 0 0,6 7 0 0 0,2 1 0 0 0,-1 5 0 0 0,-3 1 0 0 0,-2 1 0 0 0,0 3 0 0 0,0-4 0 0 0,-1-1 0 0 0,-1-2 0 0 0,1 3 0 0 0,-2-2 0 0 0,1-3 0 0 0,-4-3 0 0 0,0-5 0 0 0,-4-5 0 0 0,-2 2 0 0 0,2-6 0 0 0,3 1 0 0 0,3-4 0 0 0,-2-1 0 0 0,-3 0 0 0 0,-3-1 0 0 0,2 1 0 0 0,6 1 0 0 0,1-1 0 0 0,-4-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">20845 4727 16383 0 0,'12'0'0'0'0,"7"0"0"0"0,4 0 0 0 0,-3 3 0 0 0,1 6 0 0 0,1 4 0 0 0,-1 0 0 0 0,-1 5 0 0 0,8 23 0 0 0,6 14 0 0 0,-1 3 0 0 0,-5 0 0 0 0,-2-3 0 0 0,1-2 0 0 0,-1-1 0 0 0,-6-5 0 0 0,7 8 0 0 0,1 1 0 0 0,-4-7 0 0 0,0 0 0 0 0,-1-7 0 0 0,-4-5 0 0 0,-6-1 0 0 0,-2-9 0 0 0,0-1 0 0 0,-2-1 0 0 0,1 2 0 0 0,5 11 0 0 0,-1 3 0 0 0,7 11 0 0 0,-1 1 0 0 0,-3-5 0 0 0,1 22 0 0 0,-2-2 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">19432 6109 16383 0 0,'9'0'0'0'0,"6"0"0"0"0,4 0 0 0 0,1 0 0 0 0,3 0 0 0 0,4 0 0 0 0,3 0 0 0 0,0 0 0 0 0,1 0 0 0 0,3 0 0 0 0,3 0 0 0 0,4 0 0 0 0,-3-4 0 0 0,-1-1 0 0 0,-4 2 0 0 0,-4-2 0 0 0,1 3 0 0 0,-1 0 0 0 0,-3 1 0 0 0,-2 1 0 0 0,0-3 0 0 0,4-2 0 0 0,-2 0 0 0 0,-2 3 0 0 0,-1-1 0 0 0,-3-3 0 0 0,-3-2 0 0 0,0-1 0 0 0,1 0 0 0 0,6 0 0 0 0,5-1 0 0 0,-2 0 0 0 0,-1 1 0 0 0,-3-3 0 0 0,-4-1 0 0 0,5-2 0 0 0,1 1 0 0 0,-1 2 0 0 0,1 1 0 0 0,0 2 0 0 0,-1-2 0 0 0,-3 2 0 0 0,0-2 0 0 0,1 1 0 0 0,0 3 0 0 0,-4-1 0 0 0,-1 1 0 0 0,-2-3 0 0 0,-2 1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">20492 7093 16383 0 0,'3'0'0'0'0,"10"0"0"0"0,17 0 0 0 0,14 0 0 0 0,4 0 0 0 0,1 0 0 0 0,-3 0 0 0 0,-2 0 0 0 0,-6 0 0 0 0,-3 0 0 0 0,-6 0 0 0 0,0 0 0 0 0,6 0 0 0 0,6 0 0 0 0,5 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,7 0 0 0 0,4 0 0 0 0,1-4 0 0 0,-6-1 0 0 0,-6 2 0 0 0,-8-1 0 0 0,-5-3 0 0 0,-1 1 0 0 0,-3 0 0 0 0,2-1 0 0 0,2-4 0 0 0,2-3 0 0 0,0-2 0 0 0,0-1 0 0 0,-2 5 0 0 0,-1 0 0 0 0,0-1 0 0 0,-3-2 0 0 0,1 0 0 0 0,-6 1 0 0 0,-1-1 0 0 0,-3-2 0 0 0,-4 2 0 0 0,3 3 0 0 0,4-6 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 2 0 0 0,-1 2 0 0 0,-5 0 0 0 0,-1-3 0 0 0,-1 4 0 0 0,4-2 0 0 0,-2 1 0 0 0,0 2 0 0 0,0 2 0 0 0,3 0 0 0 0,-1-1 0 0 0,-2-2 0 0 0,-2-2 0 0 0,-1 0 0 0 0,0 4 0 0 0,4-3 0 0 0,3-3 0 0 0,0 3 0 0 0,0-6 0 0 0,-1 4 0 0 0,-3-1 0 0 0,-4 4 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36.47">26144 6988 16383 0 0,'-6'0'0'0'0,"-9"4"0"0"0,-4 1 0 0 0,-1 3 0 0 0,-5 11 0 0 0,4 9 0 0 0,4 29 0 0 0,5 18 0 0 0,8 5 0 0 0,10-13 0 0 0,8-17 0 0 0,1-13 0 0 0,4-13 0 0 0,2-11 0 0 0,0-7 0 0 0,0-6 0 0 0,0-2 0 0 0,-2 0 0 0 0,-1 0 0 0 0,1-8 0 0 0,-2-2 0 0 0,1-4 0 0 0,-4-6 0 0 0,0 0 0 0 0,0-4 0 0 0,-3-6 0 0 0,-3 0 0 0 0,-2-10 0 0 0,-3-3 0 0 0,-5 5 0 0 0,-4 9 0 0 0,-6 9 0 0 0,-8 10 0 0 0,-5 7 0 0 0,0 3 0 0 0,0 2 0 0 0,2 3 0 0 0,2-1 0 0 0,0-1 0 0 0,2 0 0 0 0,5 8 0 0 0,3 4 0 0 0,1 8 0 0 0,0 4 0 0 0,1 1 0 0 0,8 15 0 0 0,16 13 0 0 0,6 2 0 0 0,2-8 0 0 0,5-14 0 0 0,1-12 0 0 0,0-8 0 0 0,-2-9 0 0 0,-6-7 0 0 0,-3-4 0 0 0,-2-12 0 0 0,-4-12 0 0 0,6-14 0 0 0,-1-2 0 0 0,-3 4 0 0 0,-4 5 0 0 0,-4 5 0 0 0,1-3 0 0 0,-2-1 0 0 0,-1 0 0 0 0,-2 4 0 0 0,-3 6 0 0 0,-5 9 0 0 0,-8 7 0 0 0,-4 5 0 0 0,-5 2 0 0 0,-2 3 0 0 0,-2 2 0 0 0,0 0 0 0 0,1 3 0 0 0,3 1 0 0 0,5 2 0 0 0,0 5 0 0 0,-2 10 0 0 0,2 4 0 0 0,3 1 0 0 0,4 29 0 0 0,19 30 0 0 0,29 20 0 0 0,18-4 0 0 0,5-20 0 0 0,-5-23 0 0 0,-9-22 0 0 0,-8-18 0 0 0,-9-12 0 0 0,-8-11 0 0 0,-3-9 0 0 0,-4-9 0 0 0,-4-5 0 0 0,-4-8 0 0 0,0 1 0 0 0,-1-4 0 0 0,-1-7 0 0 0,1 1 0 0 0,0 4 0 0 0,0 6 0 0 0,-5-11 0 0 0,-5 4 0 0 0,-5 3 0 0 0,-6 9 0 0 0,-7 9 0 0 0,-8 9 0 0 0,-6 5 0 0 0,2 3 0 0 0,3 3 0 0 0,4 0 0 0 0,1 0 0 0 0,2 5 0 0 0,2 7 0 0 0,5 5 0 0 0,3 3 0 0 0,3 3 0 0 0,11 9 0 0 0,20 16 0 0 0,9-3 0 0 0,4-8 0 0 0,-4-9 0 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -8475,9 +8486,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8515,7 +8526,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8621,7 +8632,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8763,7 +8774,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8777,33 +8788,33 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
+    <col min="15" max="15" width="44.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="O2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="O3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -8818,7 +8829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -8836,17 +8847,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="N9" t="s">
         <v>12</v>
       </c>
@@ -8854,7 +8865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="K10" t="s">
         <v>13</v>
       </c>
@@ -8865,7 +8876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="I11" t="s">
         <v>15</v>
       </c>
@@ -8882,7 +8893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="H12" t="s">
         <v>20</v>
       </c>
@@ -8902,7 +8913,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="I13" s="1">
         <v>0</v>
       </c>
@@ -8910,11 +8921,11 @@
         <v>5</v>
       </c>
       <c r="K13">
-        <f>J13-$N$10</f>
+        <f t="shared" ref="K13:K22" si="0">J13-$N$10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="I14" s="1">
         <v>6</v>
       </c>
@@ -8922,7 +8933,7 @@
         <v>13</v>
       </c>
       <c r="K14">
-        <f>J14-$N$10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L14">
@@ -8930,7 +8941,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="1">
-        <f>I14-I13</f>
+        <f t="shared" ref="M14:M21" si="1">I14-I13</f>
         <v>6</v>
       </c>
       <c r="N14">
@@ -8942,7 +8953,7 @@
         <v>86400</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="I15" s="1">
         <v>12</v>
       </c>
@@ -8950,7 +8961,7 @@
         <v>26</v>
       </c>
       <c r="K15">
-        <f>J15-$N$10</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="L15">
@@ -8958,19 +8969,19 @@
         <v>14.5</v>
       </c>
       <c r="M15" s="1">
-        <f>I15-I14</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15:N21" si="0">M15*60*60</f>
+        <f t="shared" ref="N15:N21" si="2">M15*60*60</f>
         <v>21600</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15:O21" si="1">L15*N15</f>
+        <f t="shared" ref="O15:O21" si="3">L15*N15</f>
         <v>313200</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="I16" s="1">
         <v>18</v>
       </c>
@@ -8978,27 +8989,27 @@
         <v>21</v>
       </c>
       <c r="K16">
-        <f>J16-$N$10</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L15:L21" si="2">(K15+K16)/2</f>
+        <f t="shared" ref="L16:L21" si="4">(K15+K16)/2</f>
         <v>18.5</v>
       </c>
       <c r="M16" s="1">
-        <f>I16-I15</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>21600</v>
       </c>
       <c r="O16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>399600</v>
       </c>
     </row>
-    <row r="17" spans="7:16">
+    <row r="17" spans="7:16" x14ac:dyDescent="0.35">
       <c r="H17" t="s">
         <v>12</v>
       </c>
@@ -9009,27 +9020,27 @@
         <v>16</v>
       </c>
       <c r="K17">
-        <f>J17-$N$10</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L17">
+        <f t="shared" si="4"/>
+        <v>13.5</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="2"/>
-        <v>13.5</v>
-      </c>
-      <c r="M17" s="1">
-        <f>I17-I16</f>
-        <v>6</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="O17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>291600</v>
       </c>
     </row>
-    <row r="18" spans="7:16">
+    <row r="18" spans="7:16" x14ac:dyDescent="0.35">
       <c r="H18" t="s">
         <v>24</v>
       </c>
@@ -9040,27 +9051,27 @@
         <v>12</v>
       </c>
       <c r="K18">
-        <f>J18-$N$10</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L18">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="M18" s="1">
-        <f>I18-I17</f>
-        <v>6</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="O18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>194400</v>
       </c>
     </row>
-    <row r="19" spans="7:16">
+    <row r="19" spans="7:16" x14ac:dyDescent="0.35">
       <c r="I19" s="1">
         <v>36</v>
       </c>
@@ -9068,27 +9079,27 @@
         <v>9</v>
       </c>
       <c r="K19">
-        <f>J19-$N$10</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L19">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="2"/>
-        <v>5.5</v>
-      </c>
-      <c r="M19" s="1">
-        <f>I19-I18</f>
-        <v>6</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="O19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>118800</v>
       </c>
     </row>
-    <row r="20" spans="7:16">
+    <row r="20" spans="7:16" x14ac:dyDescent="0.35">
       <c r="I20" s="1">
         <v>42</v>
       </c>
@@ -9096,27 +9107,27 @@
         <v>7</v>
       </c>
       <c r="K20">
-        <f>J20-$N$10</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L20">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="M20" s="1">
-        <f>I20-I19</f>
-        <v>6</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="O20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>64800</v>
       </c>
     </row>
-    <row r="21" spans="7:16">
+    <row r="21" spans="7:16" x14ac:dyDescent="0.35">
       <c r="I21" s="1">
         <v>48</v>
       </c>
@@ -9124,27 +9135,27 @@
         <v>5</v>
       </c>
       <c r="K21">
-        <f>J21-$N$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M21" s="1">
-        <f>I21-I20</f>
-        <v>6</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21600</v>
       </c>
     </row>
-    <row r="22" spans="7:16">
+    <row r="22" spans="7:16" x14ac:dyDescent="0.35">
       <c r="I22">
         <v>54</v>
       </c>
@@ -9152,7 +9163,7 @@
         <v>5</v>
       </c>
       <c r="K22">
-        <f>J22-$N$10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M22">
@@ -9160,7 +9171,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="7:16">
+    <row r="23" spans="7:16" x14ac:dyDescent="0.35">
       <c r="I23">
         <v>60</v>
       </c>
@@ -9178,7 +9189,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="7:16">
+    <row r="24" spans="7:16" x14ac:dyDescent="0.35">
       <c r="I24">
         <v>66</v>
       </c>
@@ -9196,7 +9207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="7:16">
+    <row r="25" spans="7:16" x14ac:dyDescent="0.35">
       <c r="O25" t="s">
         <v>27</v>
       </c>
@@ -9204,12 +9215,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="7:16">
+    <row r="26" spans="7:16" x14ac:dyDescent="0.35">
       <c r="P26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="7:16">
+    <row r="27" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G27" t="s">
         <v>30</v>
       </c>
@@ -9231,12 +9242,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="7:16">
+    <row r="28" spans="7:16" x14ac:dyDescent="0.35">
       <c r="L28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="7:16">
+    <row r="30" spans="7:16" x14ac:dyDescent="0.35">
       <c r="L30" t="s">
         <v>35</v>
       </c>
@@ -9248,7 +9259,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="7:16">
+    <row r="31" spans="7:16" x14ac:dyDescent="0.35">
       <c r="M31" t="s">
         <v>37</v>
       </c>
@@ -9267,14 +9278,14 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="7:16">
+    <row r="2" spans="7:16" x14ac:dyDescent="0.35">
       <c r="M2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="7:16">
+    <row r="3" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G3">
         <v>0</v>
       </c>
@@ -9282,7 +9293,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="7:16">
+    <row r="4" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G4">
         <v>6</v>
       </c>
@@ -9290,22 +9301,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="7:16">
+    <row r="5" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="7:16">
+    <row r="6" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G6">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="7:16">
+    <row r="7" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G7">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="7:16">
+    <row r="8" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G8">
         <v>30</v>
       </c>
@@ -9313,25 +9324,25 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="7:16">
+    <row r="9" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G9">
         <f>G8+6</f>
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="7:16">
+    <row r="10" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G10">
         <f t="shared" ref="G10:G13" si="0">G9+6</f>
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="7:16">
+    <row r="11" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G11">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="7:16">
+    <row r="12" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G12">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -9340,7 +9351,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="7:16">
+    <row r="13" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G13">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -9354,24 +9365,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2061DDE0-6EB9-4775-A0B2-4F31BDCA142E}">
-  <dimension ref="J3:L20"/>
+  <dimension ref="J3:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="10:12">
+    <row r="3" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="10:12">
+    <row r="4" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J4" t="s">
         <v>43</v>
       </c>
@@ -9379,15 +9391,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="10:12">
+    <row r="5" spans="10:13" x14ac:dyDescent="0.35">
       <c r="K5" t="s">
         <v>45</v>
       </c>
       <c r="L5" t="s">
         <v>46</v>
       </c>
+      <c r="M5" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="6" spans="10:12">
+    <row r="6" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J6">
         <v>0</v>
       </c>
@@ -9398,8 +9413,12 @@
         <f>K6*3.5</f>
         <v>0</v>
       </c>
+      <c r="M6">
+        <f>K6*5</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="10:12">
+    <row r="7" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J7">
         <v>3</v>
       </c>
@@ -9410,8 +9429,12 @@
         <f>K7*3.5</f>
         <v>87.5</v>
       </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M20" si="0">K7*5</f>
+        <v>125</v>
+      </c>
     </row>
-    <row r="8" spans="10:12">
+    <row r="8" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J8">
         <f>J7+3</f>
         <v>6</v>
@@ -9420,63 +9443,83 @@
         <v>50</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:L20" si="0">K8*3.5</f>
+        <f t="shared" ref="L8:L20" si="1">K8*3.5</f>
         <v>175</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
     </row>
-    <row r="9" spans="10:12">
+    <row r="9" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J9">
-        <f t="shared" ref="J9:J17" si="1">J8+3</f>
+        <f t="shared" ref="J9:J12" si="2">J8+3</f>
         <v>9</v>
       </c>
       <c r="K9">
         <v>85</v>
       </c>
       <c r="L9">
+        <f t="shared" si="1"/>
+        <v>297.5</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="0"/>
-        <v>297.5</v>
+        <v>425</v>
       </c>
     </row>
-    <row r="10" spans="10:12">
+    <row r="10" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="K10">
         <v>125</v>
       </c>
       <c r="L10">
+        <f t="shared" si="1"/>
+        <v>437.5</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="0"/>
-        <v>437.5</v>
+        <v>625</v>
       </c>
     </row>
-    <row r="11" spans="10:12">
+    <row r="11" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="K11">
         <v>160</v>
       </c>
       <c r="L11">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="0"/>
-        <v>560</v>
+        <v>800</v>
       </c>
     </row>
-    <row r="12" spans="10:12">
+    <row r="12" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="K12">
         <v>185</v>
       </c>
       <c r="L12">
+        <f t="shared" si="1"/>
+        <v>647.5</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="0"/>
-        <v>647.5</v>
+        <v>925</v>
       </c>
     </row>
-    <row r="13" spans="10:12">
+    <row r="13" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J13">
         <f>J12+6</f>
         <v>24</v>
@@ -9485,63 +9528,83 @@
         <v>160</v>
       </c>
       <c r="L13">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="0"/>
-        <v>560</v>
+        <v>800</v>
       </c>
     </row>
-    <row r="14" spans="10:12">
+    <row r="14" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J14">
-        <f t="shared" ref="J14:J22" si="2">J13+6</f>
+        <f t="shared" ref="J14:J19" si="3">J13+6</f>
         <v>30</v>
       </c>
       <c r="K14">
         <v>110</v>
       </c>
       <c r="L14">
+        <f t="shared" si="1"/>
+        <v>385</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="0"/>
-        <v>385</v>
+        <v>550</v>
       </c>
     </row>
-    <row r="15" spans="10:12">
+    <row r="15" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="K15">
         <v>60</v>
       </c>
       <c r="L15">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="16" spans="10:12">
+    <row r="16" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="K16">
         <v>36</v>
       </c>
       <c r="L16">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="M16">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>180</v>
       </c>
     </row>
-    <row r="17" spans="10:12">
+    <row r="17" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="K17">
         <v>25</v>
       </c>
       <c r="L17">
+        <f t="shared" si="1"/>
+        <v>87.5</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="18" spans="10:12">
+    <row r="18" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J18">
         <f>J17+6</f>
         <v>54</v>
@@ -9550,24 +9613,32 @@
         <v>16</v>
       </c>
       <c r="L18">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="19" spans="10:12">
+    <row r="19" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="K19">
         <v>8</v>
       </c>
       <c r="L19">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="20" spans="10:12">
+    <row r="20" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J20">
         <f>J19+9</f>
         <v>69</v>
@@ -9576,6 +9647,10 @@
         <v>0</v>
       </c>
       <c r="L20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -9590,20 +9665,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425D9EDF-B419-45D6-9F6B-BF9947B4C926}">
   <dimension ref="D3:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO5" sqref="AO5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="9.140625" style="5"/>
-    <col min="9" max="9" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="5"/>
-    <col min="12" max="12" width="18.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="5"/>
+    <col min="9" max="9" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="5"/>
+    <col min="12" max="12" width="18.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:41">
+    <row r="3" spans="4:41" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>41</v>
       </c>
@@ -9623,7 +9698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="4:41">
+    <row r="4" spans="4:41" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
         <v>43</v>
       </c>
@@ -9637,7 +9712,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="4:41">
+    <row r="5" spans="4:41" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>45</v>
       </c>
@@ -9669,7 +9744,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="4:41">
+    <row r="6" spans="4:41" x14ac:dyDescent="0.35">
       <c r="D6" s="2"/>
       <c r="E6" s="6">
         <v>0</v>
@@ -9698,7 +9773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:41">
+    <row r="7" spans="4:41" x14ac:dyDescent="0.35">
       <c r="D7" s="2"/>
       <c r="E7" s="6">
         <v>3</v>
@@ -9734,7 +9809,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="4:41">
+    <row r="8" spans="4:41" x14ac:dyDescent="0.35">
       <c r="D8" s="5" t="s">
         <v>56</v>
       </c>
@@ -9756,7 +9831,7 @@
       <c r="I8" s="6">
         <v>0</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="1">
         <f>I8+6</f>
         <v>6</v>
       </c>
@@ -9787,7 +9862,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="4:41">
+    <row r="9" spans="4:41" x14ac:dyDescent="0.35">
       <c r="D9" s="3"/>
       <c r="E9" s="8">
         <f t="shared" ref="E9:E12" si="3">E8+3</f>
@@ -9807,7 +9882,7 @@
       <c r="I9" s="6">
         <v>3</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="1">
         <f t="shared" ref="J9:J14" si="4">I9+6</f>
         <v>9</v>
       </c>
@@ -9838,7 +9913,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="4:41">
+    <row r="10" spans="4:41" x14ac:dyDescent="0.35">
       <c r="D10" s="3"/>
       <c r="E10" s="8">
         <f t="shared" si="3"/>
@@ -9859,7 +9934,7 @@
         <f>I9+3</f>
         <v>6</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
@@ -9890,7 +9965,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="11" spans="4:41">
+    <row r="11" spans="4:41" x14ac:dyDescent="0.35">
       <c r="D11" s="4"/>
       <c r="E11" s="9">
         <f t="shared" si="3"/>
@@ -9911,7 +9986,7 @@
         <f t="shared" ref="I11:I14" si="7">I10+3</f>
         <v>9</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
@@ -9942,7 +10017,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="12" spans="4:41">
+    <row r="12" spans="4:41" x14ac:dyDescent="0.35">
       <c r="E12" s="1">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -9962,7 +10037,7 @@
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
@@ -9993,7 +10068,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="13" spans="4:41">
+    <row r="13" spans="4:41" x14ac:dyDescent="0.35">
       <c r="E13" s="1">
         <v>21</v>
       </c>
@@ -10005,7 +10080,7 @@
         <f t="shared" si="2"/>
         <v>1725</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <f>F13*3</f>
         <v>517.5</v>
       </c>
@@ -10013,15 +10088,15 @@
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="1">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="12">
         <f t="shared" si="5"/>
         <v>320</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="13">
         <f t="shared" si="6"/>
         <v>837.5</v>
       </c>
@@ -10044,7 +10119,7 @@
         <v>837.5</v>
       </c>
     </row>
-    <row r="14" spans="4:41">
+    <row r="14" spans="4:41" x14ac:dyDescent="0.35">
       <c r="E14" s="1">
         <f>E12+6</f>
         <v>24</v>
@@ -10064,7 +10139,7 @@
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="1">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
@@ -10095,57 +10170,57 @@
         <v>850</v>
       </c>
     </row>
-    <row r="15" spans="4:41" s="15" customFormat="1">
-      <c r="E15" s="15">
+    <row r="15" spans="4:41" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="14">
         <f t="shared" ref="E15:E20" si="8">E14+6</f>
         <v>30</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>110</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="2"/>
         <v>1100</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="14">
         <v>21</v>
       </c>
-      <c r="J15" s="10">
-        <f>I16+6</f>
+      <c r="J15" s="1">
+        <f t="shared" ref="J15:J21" si="9">I16+6</f>
         <v>30</v>
       </c>
       <c r="K15" s="5">
-        <f>F14*2</f>
+        <f t="shared" ref="K15:K21" si="10">F14*2</f>
         <v>320</v>
       </c>
-      <c r="L15" s="15">
-        <f>H15+K15</f>
+      <c r="L15" s="14">
+        <f t="shared" ref="L15:L25" si="11">H15+K15</f>
         <v>650</v>
       </c>
-      <c r="AJ15" s="15">
+      <c r="AJ15" s="14">
         <v>30</v>
       </c>
-      <c r="AK15" s="15">
+      <c r="AK15" s="14">
         <v>110</v>
       </c>
-      <c r="AL15" s="15">
+      <c r="AL15" s="14">
         <v>1100</v>
       </c>
-      <c r="AM15" s="15">
+      <c r="AM15" s="14">
         <v>330</v>
       </c>
-      <c r="AN15" s="15">
+      <c r="AN15" s="14">
         <v>320</v>
       </c>
-      <c r="AO15" s="15">
+      <c r="AO15" s="14">
         <v>650</v>
       </c>
     </row>
-    <row r="16" spans="4:41">
+    <row r="16" spans="4:41" x14ac:dyDescent="0.35">
       <c r="E16" s="1">
         <f t="shared" si="8"/>
         <v>36</v>
@@ -10165,16 +10240,16 @@
         <f>I14+6</f>
         <v>24</v>
       </c>
-      <c r="J16" s="10">
-        <f>I17+6</f>
+      <c r="J16" s="1">
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="K16" s="5">
-        <f>F15*2</f>
+        <f t="shared" si="10"/>
         <v>220</v>
       </c>
-      <c r="L16" s="15">
-        <f>H16+K16</f>
+      <c r="L16" s="14">
+        <f t="shared" si="11"/>
         <v>400</v>
       </c>
       <c r="AJ16">
@@ -10196,7 +10271,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="5:41">
+    <row r="17" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E17" s="1">
         <f t="shared" si="8"/>
         <v>42</v>
@@ -10213,19 +10288,19 @@
         <v>108</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ref="I17:I22" si="9">I16+6</f>
+        <f t="shared" ref="I17:I22" si="12">I16+6</f>
         <v>30</v>
       </c>
-      <c r="J17" s="10">
-        <f>I18+6</f>
+      <c r="J17" s="1">
+        <f t="shared" si="9"/>
         <v>42</v>
       </c>
       <c r="K17" s="5">
-        <f>F16*2</f>
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
-      <c r="L17" s="15">
-        <f>H17+K17</f>
+      <c r="L17" s="14">
+        <f t="shared" si="11"/>
         <v>228</v>
       </c>
       <c r="AJ17">
@@ -10247,7 +10322,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="5:41">
+    <row r="18" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E18" s="1">
         <f t="shared" si="8"/>
         <v>48</v>
@@ -10264,19 +10339,19 @@
         <v>75</v>
       </c>
       <c r="I18" s="1">
+        <f t="shared" si="12"/>
+        <v>36</v>
+      </c>
+      <c r="J18" s="1">
         <f t="shared" si="9"/>
-        <v>36</v>
-      </c>
-      <c r="J18" s="10">
-        <f>I19+6</f>
         <v>48</v>
       </c>
       <c r="K18" s="5">
-        <f>F17*2</f>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
-      <c r="L18" s="15">
-        <f>H18+K18</f>
+      <c r="L18" s="14">
+        <f t="shared" si="11"/>
         <v>147</v>
       </c>
       <c r="AJ18">
@@ -10298,7 +10373,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="5:41">
+    <row r="19" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E19" s="1">
         <f>E18+6</f>
         <v>54</v>
@@ -10315,19 +10390,19 @@
         <v>48</v>
       </c>
       <c r="I19" s="1">
+        <f t="shared" si="12"/>
+        <v>42</v>
+      </c>
+      <c r="J19" s="1">
         <f t="shared" si="9"/>
-        <v>42</v>
-      </c>
-      <c r="J19" s="10">
-        <f>I20+6</f>
         <v>54</v>
       </c>
       <c r="K19" s="5">
-        <f>F18*2</f>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="L19" s="15">
-        <f>H19+K19</f>
+      <c r="L19" s="14">
+        <f t="shared" si="11"/>
         <v>98</v>
       </c>
       <c r="AJ19">
@@ -10349,7 +10424,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="5:41">
+    <row r="20" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E20" s="1">
         <f t="shared" si="8"/>
         <v>60</v>
@@ -10366,19 +10441,19 @@
         <v>24</v>
       </c>
       <c r="I20" s="1">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="J20" s="1">
         <f t="shared" si="9"/>
-        <v>48</v>
-      </c>
-      <c r="J20" s="10">
-        <f>I21+6</f>
         <v>60</v>
       </c>
       <c r="K20" s="5">
-        <f>F19*2</f>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
-      <c r="L20" s="15">
-        <f>H20+K20</f>
+      <c r="L20" s="14">
+        <f t="shared" si="11"/>
         <v>56</v>
       </c>
       <c r="AJ20">
@@ -10400,7 +10475,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="5:41">
+    <row r="21" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E21" s="1">
         <v>66</v>
       </c>
@@ -10412,7 +10487,7 @@
         <f t="shared" si="2"/>
         <v>26.666666666666671</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -10420,16 +10495,16 @@
         <f>I20+6</f>
         <v>54</v>
       </c>
-      <c r="J21" s="11">
-        <f>I22+6</f>
+      <c r="J21" s="10">
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
-      <c r="K21" s="13">
-        <f>F20*2</f>
+      <c r="K21" s="12">
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
-      <c r="L21" s="15">
-        <f>H21+K21</f>
+      <c r="L21" s="14">
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
       <c r="AJ21">
@@ -10451,7 +10526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="5:41" ht="15.75">
+    <row r="22" spans="5:41" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E22" s="1">
         <f>E20+9</f>
         <v>69</v>
@@ -10463,25 +10538,25 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="12">
         <f>H21+((F22-F21)/(F23-F21))*(H23-H21)</f>
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="J22">
         <v>72</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="12">
         <v>0</v>
       </c>
-      <c r="L22" s="15">
-        <f>H22+K22</f>
+      <c r="L22" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="12" t="s">
+      <c r="Q22" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AJ22">
@@ -10503,7 +10578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="5:41">
+    <row r="23" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E23" s="1">
         <v>72</v>
       </c>
@@ -10526,8 +10601,8 @@
         <f>F22*2</f>
         <v>0</v>
       </c>
-      <c r="L23" s="15">
-        <f>H23+K23</f>
+      <c r="L23" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ23">
@@ -10546,7 +10621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="5:41">
+    <row r="24" spans="5:41" x14ac:dyDescent="0.35">
       <c r="E24" s="1">
         <f>E22+6</f>
         <v>75</v>
@@ -10573,8 +10648,8 @@
         <f>F23*2</f>
         <v>0</v>
       </c>
-      <c r="L24" s="15">
-        <f>H24+K24</f>
+      <c r="L24" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S24">
@@ -10604,7 +10679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="5:41">
+    <row r="25" spans="5:41" x14ac:dyDescent="0.35">
       <c r="G25" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -10620,8 +10695,8 @@
         <f>F24*2</f>
         <v>0</v>
       </c>
-      <c r="L25" s="15">
-        <f>H25+K25</f>
+      <c r="L25" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S25">
@@ -10638,7 +10713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:41">
+    <row r="26" spans="5:41" x14ac:dyDescent="0.35">
       <c r="G26" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -10651,13 +10726,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:41">
+    <row r="27" spans="5:41" x14ac:dyDescent="0.35">
       <c r="G27" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L27" s="15">
-        <f t="shared" ref="L27" si="10">H26+K27</f>
+      <c r="L27" s="14">
+        <f t="shared" ref="L27" si="13">H26+K27</f>
         <v>0</v>
       </c>
       <c r="AL27">

</xml_diff>